<commit_message>
Fix format of SYNoEVC file
</commit_message>
<xml_diff>
--- a/InputData/trans/SYNoEVC/Start Year Number of EV Chargers.xlsx
+++ b/InputData/trans/SYNoEVC/Start Year Number of EV Chargers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\SYNoEVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFB0A12-A899-4D93-B194-4DFB564BB149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F02A167-1F89-4FD5-AE13-9CC7B683C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -653,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -2462,8 +2462,8 @@
   </sheetPr>
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AE2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2476,220 +2476,61 @@
         <v>32</v>
       </c>
       <c r="B1">
-        <v>2021</v>
-      </c>
-      <c r="C1" s="3">
-        <v>2022</v>
-      </c>
-      <c r="D1">
-        <v>2023</v>
-      </c>
-      <c r="E1" s="3">
-        <v>2024</v>
-      </c>
-      <c r="F1">
-        <v>2025</v>
-      </c>
-      <c r="G1" s="3">
-        <v>2026</v>
-      </c>
-      <c r="H1">
-        <v>2027</v>
-      </c>
-      <c r="I1" s="3">
-        <v>2028</v>
-      </c>
-      <c r="J1">
-        <v>2029</v>
-      </c>
-      <c r="K1" s="3">
-        <v>2030</v>
-      </c>
-      <c r="L1">
-        <v>2031</v>
-      </c>
-      <c r="M1" s="3">
-        <v>2032</v>
-      </c>
-      <c r="N1">
-        <v>2033</v>
-      </c>
-      <c r="O1" s="3">
-        <v>2034</v>
-      </c>
-      <c r="P1">
-        <v>2035</v>
-      </c>
-      <c r="Q1" s="3">
-        <v>2036</v>
-      </c>
-      <c r="R1">
-        <v>2037</v>
-      </c>
-      <c r="S1" s="3">
-        <v>2038</v>
-      </c>
-      <c r="T1">
-        <v>2039</v>
-      </c>
-      <c r="U1" s="3">
-        <v>2040</v>
-      </c>
-      <c r="V1">
-        <v>2041</v>
-      </c>
-      <c r="W1" s="3">
-        <v>2042</v>
-      </c>
-      <c r="X1">
-        <v>2043</v>
-      </c>
-      <c r="Y1" s="3">
-        <v>2044</v>
-      </c>
-      <c r="Z1">
-        <v>2045</v>
-      </c>
-      <c r="AA1" s="3">
-        <v>2046</v>
-      </c>
-      <c r="AB1">
-        <v>2047</v>
-      </c>
-      <c r="AC1" s="3">
-        <v>2048</v>
-      </c>
-      <c r="AD1">
-        <v>2049</v>
-      </c>
-      <c r="AE1" s="3">
-        <v>2050</v>
-      </c>
+        <v>2020</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AE1" s="3"/>
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="2">
-        <f>Calculations!C11</f>
+        <f>Calculations!B8</f>
         <v>137902</v>
       </c>
-      <c r="C2" s="2">
-        <f>Calculations!D11</f>
-        <v>137902</v>
-      </c>
-      <c r="D2" s="2">
-        <f>Calculations!E11</f>
-        <v>251762.11802742296</v>
-      </c>
-      <c r="E2" s="2">
-        <f>Calculations!F11</f>
-        <v>364830.05288038554</v>
-      </c>
-      <c r="F2" s="2">
-        <f>Calculations!G11</f>
-        <v>479244.6991299307</v>
-      </c>
-      <c r="G2" s="2">
-        <f>Calculations!H11</f>
-        <v>595164.49341096531</v>
-      </c>
-      <c r="H2" s="2">
-        <f>Calculations!I11</f>
-        <v>647672.73524960212</v>
-      </c>
-      <c r="I2" s="2">
-        <f>Calculations!J11</f>
-        <v>702002.99838949763</v>
-      </c>
-      <c r="J2" s="2">
-        <f>Calculations!K11</f>
-        <v>758234.50114811282</v>
-      </c>
-      <c r="K2" s="2">
-        <f>Calculations!L11</f>
-        <v>816525.68016030989</v>
-      </c>
-      <c r="L2" s="2">
-        <f>Calculations!M11</f>
-        <v>876955.75374354981</v>
-      </c>
-      <c r="M2" s="2">
-        <f>Calculations!N11</f>
-        <v>914887.82517211698</v>
-      </c>
-      <c r="N2" s="2">
-        <f>Calculations!O11</f>
-        <v>952819.89660069905</v>
-      </c>
-      <c r="O2" s="2">
-        <f>Calculations!P11</f>
-        <v>990751.96802926622</v>
-      </c>
-      <c r="P2" s="2">
-        <f>Calculations!Q11</f>
-        <v>1028684.0394578334</v>
-      </c>
-      <c r="Q2" s="2">
-        <f>Calculations!R11</f>
-        <v>1066616.1108864155</v>
-      </c>
-      <c r="R2" s="2">
-        <f>Calculations!S11</f>
-        <v>1104548.1823149826</v>
-      </c>
-      <c r="S2" s="2">
-        <f>Calculations!T11</f>
-        <v>1142480.2537435498</v>
-      </c>
-      <c r="T2" s="2">
-        <f>Calculations!U11</f>
-        <v>1180412.325172117</v>
-      </c>
-      <c r="U2" s="2">
-        <f>Calculations!V11</f>
-        <v>1218344.3966006991</v>
-      </c>
-      <c r="V2" s="2">
-        <f>Calculations!W11</f>
-        <v>1256276.4680292662</v>
-      </c>
-      <c r="W2" s="2">
-        <f>Calculations!X11</f>
-        <v>1294208.5394578334</v>
-      </c>
-      <c r="X2" s="2">
-        <f>Calculations!Y11</f>
-        <v>1332140.6108864155</v>
-      </c>
-      <c r="Y2" s="2">
-        <f>Calculations!Z11</f>
-        <v>1370072.6823149826</v>
-      </c>
-      <c r="Z2" s="2">
-        <f>Calculations!AA11</f>
-        <v>1408004.7537435498</v>
-      </c>
-      <c r="AA2" s="2">
-        <f>Calculations!AB11</f>
-        <v>1445936.825172117</v>
-      </c>
-      <c r="AB2" s="2">
-        <f>Calculations!AC11</f>
-        <v>1483868.8966006991</v>
-      </c>
-      <c r="AC2" s="2">
-        <f>Calculations!AD11</f>
-        <v>1521800.9680292662</v>
-      </c>
-      <c r="AD2" s="2">
-        <f>Calculations!AE11</f>
-        <v>1559733.0394578334</v>
-      </c>
-      <c r="AE2" s="2">
-        <f>Calculations!AF11</f>
-        <v>1597665.1108864155</v>
-      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
     </row>
   </sheetData>

</xml_diff>